<commit_message>
Notebook with code for line 77-82 added
</commit_message>
<xml_diff>
--- a/Data/Deposits report template1.xlsx
+++ b/Data/Deposits report template1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tonikph-my.sharepoint.com/personal/dchakroborti_tonikbank_com/Documents/MyStuff/Mila/Deposit Report/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3DBC82B-1947-43E2-B93E-B3073F98125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{C3DBC82B-1947-43E2-B93E-B3073F98125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C90461C-8FD1-4391-A2CD-661BA1FEEBA2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F1A1A290-985C-8B49-BDBB-ECA77596E9C6}"/>
   </bookViews>
@@ -847,15 +847,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6054C368-EFD4-9943-AA9C-937855BEFA47}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.875" customWidth="1"/>
-    <col min="2" max="2" width="29.125" customWidth="1"/>
-    <col min="3" max="3" width="49" customWidth="1"/>
+    <col min="1" max="1" width="71.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="239" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1523,7 +1523,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the query and Data Files
</commit_message>
<xml_diff>
--- a/Data/Deposits report template1.xlsx
+++ b/Data/Deposits report template1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tonikph-my.sharepoint.com/personal/dchakroborti_tonikbank_com/Documents/MyStuff/Mila/Deposit Report/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C3DBC82B-1947-43E2-B93E-B3073F98125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C90461C-8FD1-4391-A2CD-661BA1FEEBA2}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{C3DBC82B-1947-43E2-B93E-B3073F98125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6BA5CF8-7552-4D95-8092-4118834B0362}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F1A1A290-985C-8B49-BDBB-ECA77596E9C6}"/>
   </bookViews>
@@ -427,7 +427,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -461,6 +461,21 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -488,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,7 +511,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,7 +864,7 @@
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:B82"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1398,7 +1414,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="8" t="s">
         <v>95</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -1414,7 +1430,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B81" s="4" t="s">

</xml_diff>